<commit_message>
Common function implemented for Log and Extent messages
</commit_message>
<xml_diff>
--- a/Data/Result/ResNewPolicy.xlsx
+++ b/Data/Result/ResNewPolicy.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>TestId</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>GL202112301151</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>GL202112301200</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>